<commit_message>
Mise à jour du dashboard et des fichiers Excel
</commit_message>
<xml_diff>
--- a/Dashboard_Securite.xlsx
+++ b/Dashboard_Securite.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iweof-my.sharepoint.com/personal/ousmane_faye_ingka_ikea_com/Documents/Desktop/projets evolutifs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wizards station\Desktop\Projet IKEA\dashboard_securite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="534" documentId="8_{517913A8-80DD-48EC-9EF6-A5765D221831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6237D9BB-916D-42B0-8108-72A2412A91C3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECED5AE-8A73-47FD-BD5A-B8B473945C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Données" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Données!$E$1:$E$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Données!$E$9:$E$300</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Données!$E$1:$E$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Données!$E$9:$E$300</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -24,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -500,6 +504,743 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Distribution des prix</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1500" b="1" i="0" u="none" strike="noStrike" cap="all" spc="100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Distribution des prix</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{9C4DEC24-0718-4FBB-906F-7C7771D23492}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v> prix   N/A   N/A   N/A   N/A   N/A   N/A   N/A </cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{525CA465-C276-47E9-AD11-878A3CFDA7D2}">
+          <cx:axisId val="2"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="370">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" spc="100">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1101913</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>115049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1206501</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>56778</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Graphique 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C94FC09B-5561-1D3D-7C88-ACDFF3F6F93F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4314266" y="10140578"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-CA" sz="1100"/>
+                <a:t>Ce graphique n’est pas disponible dans votre version d’Excel.
+La modification de cette forme ou l’enregistrement de ce classeur dans un autre format de fichier endommagera le graphique de façon irréparable.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,15 +1544,77 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="525" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="525" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1CE86E73-900A-4DA5-8402-116E83A77DF4}">
+  <we:reference id="wa200005502" version="1.0.0.12" store="fr-FR" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200005502" version="1.0.0.12" store="WA200005502" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="docId" value="&quot;eIgwAk2PtquD4NqDBLNW0&quot;"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CREATE_PROMPT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_LIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_HLIST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CLASSIFY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TRANSLATE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_EXTRACT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TAG</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_CONVERT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_FORMAT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_SUMMARIZE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_TABLE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_FILL</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_SPLIT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_HSPLIT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_EDIT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_MATCH</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_VISION</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_GPT_WEB</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{E0CB8C45-380C-4EE9-A7B8-8A22228CCE9C}">
+  <we:reference id="wa200005669" version="2.0.0.0" store="fr-FR" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200005669" version="2.0.0.0" store="WA200005669" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="69" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -819,16 +1622,16 @@
     <col min="4" max="4" width="20" style="14" customWidth="1"/>
     <col min="5" max="5" width="20" style="9" customWidth="1"/>
     <col min="6" max="6" width="24" style="11" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="32.453125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="29.7265625" style="5" customWidth="1"/>
     <col min="9" max="9" width="40" style="5" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="23.7265625" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" style="5" customWidth="1"/>
     <col min="14" max="14" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -857,7 +1660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -886,7 +1689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2">
         <v>0.59027777777777779</v>
       </c>
@@ -912,7 +1715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>0.625</v>
       </c>
@@ -941,7 +1744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="58" x14ac:dyDescent="0.65">
       <c r="B5" s="2">
         <v>0.64583333333333337</v>
       </c>
@@ -973,7 +1776,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>0.64583333333333337</v>
       </c>
@@ -1002,7 +1805,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <v>0.6875</v>
       </c>
@@ -1031,7 +1834,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1063,7 +1866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
@@ -1092,7 +1895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>0.60416666666666663</v>
       </c>
@@ -1118,7 +1921,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>0.60416666666666663</v>
       </c>
@@ -1144,7 +1947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>0.60416666666666663</v>
       </c>
@@ -1170,7 +1973,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>0.60416666666666663</v>
       </c>
@@ -1196,7 +1999,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <v>0.77777777777777779</v>
       </c>
@@ -1222,7 +2025,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -1251,7 +2054,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>0.56666666666666665</v>
       </c>
@@ -1277,7 +2080,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>0.59930555555555554</v>
       </c>
@@ -1303,7 +2106,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>0.59930555555555554</v>
       </c>
@@ -1329,7 +2132,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>0.59930555555555554</v>
       </c>
@@ -1355,7 +2158,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>0.61041666666666672</v>
       </c>
@@ -1381,7 +2184,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>0.61041666666666672</v>
       </c>
@@ -1407,7 +2210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>0.62152777777777779</v>
       </c>
@@ -1433,7 +2236,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>0.63611111111111107</v>
       </c>
@@ -1459,7 +2262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>0.63611111111111107</v>
       </c>
@@ -1485,7 +2288,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>68</v>
       </c>
@@ -1514,7 +2317,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B26" s="2">
         <v>0.61597222222222225</v>
       </c>
@@ -1540,7 +2343,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" s="2">
         <v>0.61597222222222225</v>
       </c>
@@ -1566,7 +2369,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B28" s="2">
         <v>0.61597222222222225</v>
       </c>
@@ -1592,7 +2395,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" s="2">
         <v>0.625</v>
       </c>
@@ -1618,7 +2421,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>75</v>
       </c>
@@ -1647,7 +2450,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" s="2">
         <v>0.55555555555555558</v>
       </c>
@@ -1673,7 +2476,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B32" s="2">
         <v>0.58263888888888893</v>
       </c>
@@ -1699,7 +2502,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="2">
         <v>0.59375</v>
       </c>
@@ -1725,824 +2528,838 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C35" s="17"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C36" s="17"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C37" s="17"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C40" s="17"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C41" s="17"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C42" s="17"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C43" s="17"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C44" s="17"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C45" s="17"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C46" s="17"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C47" s="17"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C48" s="17"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" s="17"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" s="17"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" s="17"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" s="17"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" s="17"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" s="17"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" s="17"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" s="17"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" s="17"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" s="17"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" s="17"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" s="17"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" s="17"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" s="17"/>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" s="17"/>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" s="17"/>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" s="17"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" s="17"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="17"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" s="17"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" s="17"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" s="17"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="17"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72" s="17"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" s="17"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74" s="17"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75" s="17"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76" s="17"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" s="17"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78" s="17"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79" s="17"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80" s="17"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" s="17"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" s="17"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" s="17"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" s="17"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" s="17"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="17"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="17"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="17"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="17"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" s="17"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="17"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" s="17"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="17"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="17"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="17"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="17"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="17"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" s="17"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" s="17"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C100" s="17"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101" s="17"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C102" s="17"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C103" s="17"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C104" s="17"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C105" s="17"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C106" s="17"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107" s="17"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" s="17"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C109" s="17"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110" s="17"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111" s="17"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" s="17"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" s="17"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114" s="17"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115" s="17"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116" s="17"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117" s="17"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C118" s="17"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119" s="17"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C120" s="17"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121" s="17"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C122" s="17"/>
     </row>
-    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C123" s="17"/>
     </row>
-    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C124" s="17"/>
     </row>
-    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C125" s="17"/>
     </row>
-    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C126" s="17"/>
     </row>
-    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C127" s="17"/>
     </row>
-    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C128" s="17"/>
     </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" s="17"/>
     </row>
-    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C130" s="17"/>
     </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C131" s="17"/>
     </row>
-    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C132" s="17"/>
     </row>
-    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C133" s="17"/>
     </row>
-    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C134" s="17"/>
     </row>
-    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C135" s="17"/>
     </row>
-    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C136" s="17"/>
     </row>
-    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C137" s="17"/>
     </row>
-    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C138" s="17"/>
     </row>
-    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C139" s="17"/>
     </row>
-    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C140" s="17"/>
     </row>
-    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C141" s="17"/>
     </row>
-    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C142" s="17"/>
     </row>
-    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C143" s="17"/>
     </row>
-    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C144" s="17"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" s="17"/>
     </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C146" s="17"/>
     </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C147" s="17"/>
     </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C148" s="17"/>
     </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C149" s="17"/>
     </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C150" s="17"/>
     </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C151" s="17"/>
     </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C152" s="17"/>
     </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C153" s="17"/>
     </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C154" s="17"/>
     </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C155" s="17"/>
     </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C156" s="17"/>
     </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C157" s="17"/>
     </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C158" s="17"/>
     </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C159" s="17"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C160" s="17"/>
     </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C161" s="17"/>
     </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C162" s="17"/>
     </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C163" s="17"/>
     </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C164" s="17"/>
     </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C165" s="17"/>
     </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C166" s="17"/>
     </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C167" s="17"/>
     </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C168" s="17"/>
     </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C169" s="17"/>
     </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C170" s="17"/>
     </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C171" s="17"/>
     </row>
-    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C172" s="17"/>
     </row>
-    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C173" s="17"/>
     </row>
-    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C174" s="17"/>
     </row>
-    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C175" s="17"/>
     </row>
-    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C176" s="17"/>
     </row>
-    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C177" s="17"/>
     </row>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C178" s="17"/>
     </row>
-    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C179" s="17"/>
     </row>
-    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C180" s="17"/>
     </row>
-    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C181" s="17"/>
     </row>
-    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C182" s="17"/>
     </row>
-    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C183" s="17"/>
     </row>
-    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C184" s="17"/>
     </row>
-    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C185" s="17"/>
     </row>
-    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C186" s="17"/>
     </row>
-    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C187" s="17"/>
     </row>
-    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C188" s="17"/>
     </row>
-    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C189" s="17"/>
     </row>
-    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C190" s="17"/>
     </row>
-    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C191" s="17"/>
     </row>
-    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C192" s="17"/>
     </row>
-    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C193" s="17"/>
     </row>
-    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C194" s="17"/>
     </row>
-    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C195" s="17"/>
     </row>
-    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C196" s="17"/>
     </row>
-    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C197" s="17"/>
     </row>
-    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C198" s="17"/>
     </row>
-    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C199" s="17"/>
     </row>
-    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C200" s="17"/>
     </row>
-    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C201" s="17"/>
     </row>
-    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C202" s="17"/>
     </row>
-    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C203" s="17"/>
     </row>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C204" s="17"/>
     </row>
-    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C205" s="17"/>
     </row>
-    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C206" s="17"/>
     </row>
-    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C207" s="17"/>
     </row>
-    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C208" s="17"/>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C209" s="17"/>
     </row>
-    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C210" s="17"/>
     </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C211" s="17"/>
     </row>
-    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C212" s="17"/>
     </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C213" s="17"/>
     </row>
-    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C214" s="17"/>
     </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C215" s="17"/>
     </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C216" s="17"/>
     </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C217" s="17"/>
     </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C218" s="17"/>
     </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C219" s="17"/>
     </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C220" s="17"/>
     </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C221" s="17"/>
     </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C222" s="17"/>
     </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C223" s="17"/>
     </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C224" s="17"/>
     </row>
-    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C225" s="17"/>
     </row>
-    <row r="226" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C226" s="17"/>
     </row>
-    <row r="227" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C227" s="17"/>
     </row>
-    <row r="228" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C228" s="17"/>
     </row>
-    <row r="229" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C229" s="17"/>
     </row>
-    <row r="230" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C230" s="17"/>
     </row>
-    <row r="231" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C231" s="17"/>
     </row>
-    <row r="232" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C232" s="17"/>
     </row>
-    <row r="233" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C233" s="17"/>
     </row>
-    <row r="234" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C234" s="17"/>
     </row>
-    <row r="235" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C235" s="17"/>
     </row>
-    <row r="236" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C236" s="17"/>
     </row>
-    <row r="237" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C237" s="17"/>
     </row>
-    <row r="238" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C238" s="17"/>
     </row>
-    <row r="239" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C239" s="17"/>
     </row>
-    <row r="240" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C240" s="17"/>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C241" s="17"/>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C242" s="17"/>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C243" s="17"/>
     </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C244" s="17"/>
     </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C245" s="17"/>
     </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C246" s="17"/>
     </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C247" s="17"/>
     </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C248" s="17"/>
     </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C249" s="17"/>
     </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C250" s="17"/>
     </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C251" s="17"/>
     </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C252" s="17"/>
     </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C253" s="17"/>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C254" s="17"/>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C255" s="17"/>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C256" s="17"/>
     </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C257" s="17"/>
     </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C258" s="17"/>
     </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C259" s="17"/>
     </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C260" s="17"/>
     </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C261" s="17"/>
     </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C262" s="17"/>
     </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C263" s="17"/>
     </row>
-    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C264" s="17"/>
     </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C265" s="17"/>
     </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C266" s="17"/>
     </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C267" s="17"/>
     </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C268" s="17"/>
     </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C269" s="17"/>
     </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C270" s="17"/>
     </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C271" s="17"/>
     </row>
-    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C272" s="17"/>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C273" s="17"/>
     </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C274" s="17"/>
     </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C275" s="17"/>
     </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C276" s="17"/>
     </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C277" s="17"/>
     </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C278" s="17"/>
     </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C279" s="17"/>
     </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C280" s="17"/>
     </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C281" s="17"/>
     </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C282" s="17"/>
     </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C283" s="17"/>
     </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C284" s="17"/>
     </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C285" s="17"/>
     </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C286" s="17"/>
     </row>
-    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C287" s="17"/>
     </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C288" s="17"/>
     </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C289" s="17"/>
     </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C290" s="17"/>
     </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C291" s="17"/>
     </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C292" s="17"/>
     </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C293" s="17"/>
     </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C294" s="17"/>
     </row>
-    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C295" s="17"/>
     </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C296" s="17"/>
     </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C297" s="17"/>
     </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C298" s="17"/>
     </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C299" s="17"/>
     </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C300" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="F2:H3 F4 H4 M4:M8 F5:H9 H10:I10 F10:F13 I11:I13 F14:H300">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>EXACT(F2,"Vol confirmé")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>EXACT(F2,"Presque vol (tentative)")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" dxfId="2" priority="10">
       <formula>EXACT(F2,"Comportement suspect")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>EXACT(F2,"Infraction procédure")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>EXACT(F2,"Autre")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E300">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFD6007B"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1E31BD46-D774-4319-BC5D-01D19AEF02F7}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2554,8 +3371,26 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1E31BD46-D774-4319-BC5D-01D19AEF02F7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E2:E300</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>